<commit_message>
Implemented generating of the "total employees" report; added icons for reports.
</commit_message>
<xml_diff>
--- a/Staffinfo.Reports/Templates/Total_Employees.xlsx
+++ b/Staffinfo.Reports/Templates/Total_Employees.xlsx
@@ -51,7 +51,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -59,7 +59,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -223,25 +223,31 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -554,7 +560,7 @@
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,40 +574,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added pdf-version of the 'total employees' report.
</commit_message>
<xml_diff>
--- a/Staffinfo.Reports/Templates/Total_Employees.xlsx
+++ b/Staffinfo.Reports/Templates/Total_Employees.xlsx
@@ -242,13 +242,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +560,7 @@
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>